<commit_message>
fix invoice calculations, update values
</commit_message>
<xml_diff>
--- a/test files/Cairo express travel 23-24- Siva.xlsx
+++ b/test files/Cairo express travel 23-24- Siva.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vscoded\Credit_App\Credit_app_v3_test\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC93384-3D3F-4DF0-A2F2-51AF669A8396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86280924-04C2-46CC-8A1F-E8FFD9BBFF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="statment" sheetId="6" r:id="rId1"/>
@@ -1058,7 +1058,7 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1361,6 +1361,9 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15">
+      <c r="A7" s="30">
+        <v>44194</v>
+      </c>
       <c r="B7" s="34">
         <v>8091478</v>
       </c>
@@ -4319,6 +4322,11 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:O66" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="notEqual" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{BFB014CB-32F7-4B29-B6B1-AA2672F47959}">
+      <formula1>A7</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>